<commit_message>
Wrote and tested subroutine matrixTools::add_seq_lengths_to_matrix_from_fasta
It takes a matrix where each row represents a genomic feature and computes adds as a column the length of the sequences corresponding to
each feature (computed from a specified fasta file).
Usage information has been added to Scripts_and_functions.xlsx
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="480">
   <si>
     <t xml:space="preserve">Subroutine</t>
   </si>
@@ -1356,6 +1356,21 @@
   </si>
   <si>
     <t xml:space="preserve">Writes a table (matrix) to a file as a list (one element on each line, e.g. 'row1_ele1, $row1_ele2, $row2_ele1, $row2_ele2, $row3_ele1...')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_seq_lengths_to_matrix_from_fasta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my @matrix=matrixTools::add_seq_lengths_to_matrix_from_fasta($file_or_var, $filename_or_matrixref, $id_col, $header_y_n, $fasta_file);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Takes a matrix (as a csv file – set $file_or_var to ‘file’ - or matrix reference – set $file_or_var to ‘var’ - where each row represents a genomic feature (e.g. a gene or transcript and a specified column is a feature ID)) and a fasta file containing the DNA/RNA/protein sequence of the features in the matrix. Using the fasta file the subroutine computes the length of each feature in the matrix, and attaches these lengths to the matrix as a new column. Set $header_y_n to ‘y’ if the original matrix has a header, otherwise to ‘n’. If the matrix was read from a csv file, the new matrix will also be printed to a csv file (as well as being returned as a matrix).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text::trim, fileTools::read_table, fastaTools::get_seq_lengths_from_fasta, fileTools::write_table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a csv file (sometimes)</t>
   </si>
   <si>
     <t xml:space="preserve">Script_name</t>
@@ -1707,10 +1722,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4490,6 +4505,32 @@
         <v>206</v>
       </c>
       <c r="H105" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="H106" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4534,7 +4575,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4552,10 +4593,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4565,22 +4606,22 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4588,25 +4629,25 @@
     </row>
     <row r="3" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>456</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>450</v>
-      </c>
       <c r="F3" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>457</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>452</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>385</v>
@@ -4614,22 +4655,22 @@
     </row>
     <row r="4" customFormat="false" ht="38.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>
@@ -4637,22 +4678,22 @@
     </row>
     <row r="5" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>385</v>
@@ -4660,22 +4701,22 @@
     </row>
     <row r="6" customFormat="false" ht="255.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>16</v>
@@ -4719,7 +4760,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4737,10 +4778,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4750,16 +4791,16 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4767,16 +4808,16 @@
     </row>
     <row r="3" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Added usage information for 'maintenance/commit_to_other_repo.pl' to 'Scripts_and_functions.xlsx'
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Subroutines" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="484">
   <si>
     <t xml:space="preserve">Subroutine</t>
   </si>
@@ -1464,6 +1464,18 @@
   </si>
   <si>
     <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commit_to_other_repo.pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perl commit_to_other_repo.pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this script if you want to apply an update of a file in this repository to a corresponding file (with the same name) in one or more different repositories. The script uses the file "commit_messages.txt" for information about which file to update in which repositories, whether to add, update or delete the file and which commit message to use.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FindBin, envir::timestamp, misc::read_list, text::trim, git, File::Copy</t>
   </si>
 </sst>
 </file>
@@ -1724,7 +1736,7 @@
   </sheetPr>
   <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
     </sheetView>
   </sheetViews>
@@ -4738,10 +4750,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4823,6 +4835,26 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>457</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updated entry for matrixTools::apply in Scripts_and_functions.xlsx
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Subroutines" sheetId="1" state="visible" r:id="rId2"/>
@@ -93,7 +93,7 @@
     <t xml:space="preserve">my @values=matrixTools::apply(\@matrix, $row_or_col, $function);</t>
   </si>
   <si>
-    <t xml:space="preserve">Applies a function (mean, median, min, max) to all rows ($row_or_col=”row”) or columns ($row_or_col=”col”) in a matrix and returns the resulting values as an array.</t>
+    <t xml:space="preserve">Applies a function ('mean', 'median', 'min', 'max', 'geomean' (geometric mean), 'stdev', 'variance') to all rows ($row_or_col=”row”) or columns ($row_or_col=”col”) in a matrix and returns the resulting values as an array.</t>
   </si>
   <si>
     <t xml:space="preserve">@array</t>
@@ -1736,8 +1736,8 @@
   </sheetPr>
   <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1839,7 +1839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" s="11" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="11" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
@@ -4568,7 +4568,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="D4 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4752,8 +4752,8 @@
   </sheetPr>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="D4 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added usage information for stats::covariance to Scripts_and_functions.xlsx
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="488">
   <si>
     <t xml:space="preserve">Subroutine</t>
   </si>
@@ -1371,6 +1371,18 @@
   </si>
   <si>
     <t xml:space="preserve">a csv file (sometimes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covariance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my $covariance=stats::covariance($arrayeref1, @arrayref2);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computes the covariance between two sets of numbers (specified as array references). The two sets must have the same number of numbers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$number</t>
   </si>
   <si>
     <t xml:space="preserve">Script_name</t>
@@ -1734,10 +1746,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L106"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4543,6 +4555,32 @@
         <v>448</v>
       </c>
       <c r="H106" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H107" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4568,7 +4606,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="D4 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4587,7 +4625,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4605,10 +4643,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4618,22 +4656,22 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4641,25 +4679,25 @@
     </row>
     <row r="3" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>459</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="F3" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>461</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>455</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>462</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>457</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>385</v>
@@ -4667,22 +4705,22 @@
     </row>
     <row r="4" customFormat="false" ht="38.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>
@@ -4690,22 +4728,22 @@
     </row>
     <row r="5" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>385</v>
@@ -4713,22 +4751,22 @@
     </row>
     <row r="6" customFormat="false" ht="255.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>16</v>
@@ -4753,7 +4791,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="D4 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4772,7 +4810,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4790,10 +4828,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4803,16 +4841,16 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4820,16 +4858,16 @@
     </row>
     <row r="3" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>16</v>
@@ -4837,19 +4875,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Updated entries for stats::variance and stats::stdev in Scripts_and_functions.xlsx (these functions now take an additional parameter)
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -1316,10 +1316,10 @@
     <t xml:space="preserve">variance</t>
   </si>
   <si>
-    <t xml:space="preserve">my $variance=stats::variance($array_ref);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Returns the sample (not population) variance of a set of numbers</t>
+    <t xml:space="preserve">my $variance=stats::variance($array_ref, $samp_or_pop);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Returns the variance of a set of numbers, specified as an array reference. Also specify whether to compute the sample variance (set $samp_or_pop = “samp”) or the population variance ( $samp_or_pop = “pop”).</t>
   </si>
   <si>
     <t xml:space="preserve">text::trim, stats::mean</t>
@@ -1748,8 +1748,8 @@
   </sheetPr>
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4428,7 +4428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>429</v>
       </c>

</xml_diff>

<commit_message>
Updated entries for stats::covariance and stats::corr_coeff in Scripts_and_functions.xlsx
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="492">
   <si>
     <t xml:space="preserve">Subroutine</t>
   </si>
@@ -1133,7 +1133,7 @@
     <t xml:space="preserve">stdev</t>
   </si>
   <si>
-    <t xml:space="preserve">my $stdev=stats::stdev($array_ref);</t>
+    <t xml:space="preserve">my $stdev=stats::stdev($array_ref, $samp_or_pop);</t>
   </si>
   <si>
     <t xml:space="preserve">Returns the sample (not population) standard deviatrion of a set of numbers</t>
@@ -1376,13 +1376,25 @@
     <t xml:space="preserve">covariance</t>
   </si>
   <si>
-    <t xml:space="preserve">my $covariance=stats::covariance($arrayeref1, @arrayref2);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computes the covariance between two sets of numbers (specified as array references). The two sets must have the same number of numbers.</t>
+    <t xml:space="preserve">my $covariance=stats::covariance($arrayeref1, $arrayref2, $samp_or_pop);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computes the covariance between two sets of numbers (specified as array references). The two sets must have the same number of numbers. Specify whether the sample or population covariance should be computed (set $samp_or_pop to ‘samp’ or ‘pop’ respectively).</t>
   </si>
   <si>
     <t xml:space="preserve">$number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corr_coeff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my $corr_coeff=stats::corr_coeff($arrayeref1, $arrayref2, $samp_or_pop);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computes the correlation coefficient between two sets of numbers (specified as array references). The two sets must have the same number of numbers. Specify whether the sample or population correlation coefficient should be computed (set $samp_or_pop to ‘samp’ or ‘pop’ respectively). Currently, the Pearson Product Moment Correlation Coefficient is the one returned, but more options (e.g. Spearman) should be added in the future.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text::trim, stats::stdev, stats::covariance</t>
   </si>
   <si>
     <t xml:space="preserve">Script_name</t>
@@ -1746,10 +1758,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A108" activeCellId="0" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4558,7 +4570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
         <v>449</v>
       </c>
@@ -4572,7 +4584,7 @@
         <v>451</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>13</v>
+        <v>432</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>452</v>
@@ -4581,6 +4593,32 @@
         <v>15</v>
       </c>
       <c r="H107" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H108" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4625,7 +4663,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4643,10 +4681,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4656,22 +4694,22 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4679,25 +4717,25 @@
     </row>
     <row r="3" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>463</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="F3" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>465</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>459</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>466</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>461</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>385</v>
@@ -4705,22 +4743,22 @@
     </row>
     <row r="4" customFormat="false" ht="38.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>
@@ -4728,22 +4766,22 @@
     </row>
     <row r="5" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>385</v>
@@ -4751,22 +4789,22 @@
     </row>
     <row r="6" customFormat="false" ht="255.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>16</v>
@@ -4810,7 +4848,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4828,10 +4866,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4841,16 +4879,16 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4858,16 +4896,16 @@
     </row>
     <row r="3" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>16</v>
@@ -4875,19 +4913,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Updated entry for subroutine listTools::value_in_array in Scripts_and_functions.xlsx
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -1307,10 +1307,10 @@
     <t xml:space="preserve">value_in_array</t>
   </si>
   <si>
-    <t xml:space="preserve">my $y_n=combinatorics::value_in_array($value, $arrayref, $num_or_char);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checks whether a value (supplied as a scalar) is present in array (supplied as an array reference) or not. Returns “y” if it is and “n” if it isn’t. Set argument $num_or_char to ‘num’ if the value and array are numeric or ‘to char’ if they are text.</t>
+    <t xml:space="preserve">my $tf=listTools::value_in_array($value, $arrayref, $num_or_char);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checks whether a value (supplied as a scalar) is present in array (supplied as an array reference) or not. Returns “TRUE” if it is and “” (an empty string) if it isn’t. Set argument $num_or_char to ‘num’ if the value and array are numeric or ‘to char’ if they are text.</t>
   </si>
   <si>
     <t xml:space="preserve">variance</t>
@@ -1761,7 +1761,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A108" activeCellId="0" sqref="A108"/>
+      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4419,7 +4419,7 @@
         <v>426</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>427</v>

</xml_diff>

<commit_message>
Added usage message for Perl subroutine stats::pearson_corr to Scripts_and_functions.xlsx
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="496">
   <si>
     <t xml:space="preserve">Subroutine</t>
   </si>
@@ -1395,6 +1395,18 @@
   </si>
   <si>
     <t xml:space="preserve">text::trim, stats::stdev, stats::covariance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pearson_corr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my $pearson_corr=stats::pearson_corr($arrayeref1, $arrayref2, $samp_or_pop);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computes the Pearson Product Moment Correlation Coefficient between two sets of numbers (specified as array references). The two sets must have the same number of numbers. Specify whether the sample or population correlation coefficient should be computed (set $samp_or_pop to ‘samp’ or ‘pop’ respectively). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">text::trim, listTools::value_in_array, stats::stdev, stats::covariance</t>
   </si>
   <si>
     <t xml:space="preserve">Script_name</t>
@@ -1758,10 +1770,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L108"/>
+  <dimension ref="A1:L109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
+      <selection pane="topLeft" activeCell="A109" activeCellId="0" sqref="109:109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4619,6 +4631,32 @@
         <v>15</v>
       </c>
       <c r="H108" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H109" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4644,7 +4682,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="109:109 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4663,7 +4701,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4681,10 +4719,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4694,22 +4732,22 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4717,25 +4755,25 @@
     </row>
     <row r="3" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="F3" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>469</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>463</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>470</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>465</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>385</v>
@@ -4743,22 +4781,22 @@
     </row>
     <row r="4" customFormat="false" ht="38.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>
@@ -4766,22 +4804,22 @@
     </row>
     <row r="5" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>385</v>
@@ -4789,22 +4827,22 @@
     </row>
     <row r="6" customFormat="false" ht="255.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>16</v>
@@ -4829,7 +4867,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="109:109 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4848,7 +4886,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4866,10 +4904,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4879,16 +4917,16 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4896,16 +4934,16 @@
     </row>
     <row r="3" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>16</v>
@@ -4913,19 +4951,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Added usage information for envir::check_arg to Scripts_and_functions.xlsx
</commit_message>
<xml_diff>
--- a/Scripts_and_functions.xlsx
+++ b/Scripts_and_functions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="501">
   <si>
     <t xml:space="preserve">Subroutine</t>
   </si>
@@ -1407,6 +1407,21 @@
   </si>
   <si>
     <t xml:space="preserve">text::trim, listTools::value_in_array, stats::stdev, stats::covariance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check_arg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my $error_message=envir::check_arg($argument, [type1, type2...], [value1, value2...]);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validates user input to scripts and functions. Returns false if everything is ok, and an error message otherwise (The decision to terminate processing lies in the script that calls this subroutine, rather than in the subroutine itself). (argument = the argument that should be validated. If argument is 0, set to 'zero')--(type = the argument's type. Options: "arrayref", "matrixref", "string", "number")--(value = a value that the argument can take. If not relevant, leave blank)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text::trim, misc::type,listTools::value_in_array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$error_message or FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">Script_name</t>
@@ -1770,10 +1785,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A109" activeCellId="0" sqref="109:109"/>
+      <selection pane="topLeft" activeCell="A110" activeCellId="0" sqref="110:110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4659,6 +4674,36 @@
       <c r="H109" s="1" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="110" s="11" customFormat="true" ht="38.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="G110" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H110" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" s="10"/>
+      <c r="J110" s="10"/>
+      <c r="K110" s="10"/>
+      <c r="L110" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4682,7 +4727,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="109:109 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="110:110 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4701,7 +4746,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4719,10 +4764,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4732,22 +4777,22 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4755,25 +4800,25 @@
     </row>
     <row r="3" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>472</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>473</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>467</v>
-      </c>
       <c r="F3" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>474</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>469</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>385</v>
@@ -4781,22 +4826,22 @@
     </row>
     <row r="4" customFormat="false" ht="38.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>
@@ -4804,22 +4849,22 @@
     </row>
     <row r="5" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>385</v>
@@ -4827,22 +4872,22 @@
     </row>
     <row r="6" customFormat="false" ht="255.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>346</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>16</v>
@@ -4867,7 +4912,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="109:109 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="110:110 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4886,7 +4931,7 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>2</v>
@@ -4904,10 +4949,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>7</v>
@@ -4917,16 +4962,16 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>16</v>
@@ -4934,16 +4979,16 @@
     </row>
     <row r="3" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>16</v>
@@ -4951,19 +4996,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>16</v>

</xml_diff>